<commit_message>
changed to only homeoffice/special occasions
</commit_message>
<xml_diff>
--- a/Arbeitszeitnachweis Vorlage.xlsx
+++ b/Arbeitszeitnachweis Vorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaa\Documents\Orga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaa\Documents\work_timer_deta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11A547A-E16E-4F4F-85CE-58050679E800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18880791-7418-457A-BBB9-1E413582109C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B46B011-59B1-4C45-95D9-6BA23A8D48A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B46B011-59B1-4C45-95D9-6BA23A8D48A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -719,7 +719,7 @@
   <dimension ref="A1:P497"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +874,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="6"/>
       <c r="I7" s="11" t="str">
-        <f>IF(F7&lt;&gt;"","Plagwitz","")</f>
+        <f>IF(F7&lt;&gt;"","Homeoffice","")</f>
         <v/>
       </c>
       <c r="J7" s="1"/>
@@ -898,7 +898,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="6"/>
       <c r="I8" s="11" t="str">
-        <f t="shared" ref="I8:I37" si="1">IF(F8&lt;&gt;"","Plagwitz","")</f>
+        <f t="shared" ref="I8:I36" si="1">IF(F8&lt;&gt;"","Homeoffice","")</f>
         <v/>
       </c>
       <c r="J8" s="1"/>
@@ -1594,7 +1594,7 @@
       <c r="G37" s="12"/>
       <c r="H37" s="13"/>
       <c r="I37" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(F37&lt;&gt;"","Homeoffice","")</f>
         <v/>
       </c>
       <c r="J37" s="1"/>

</xml_diff>

<commit_message>
updated emptiness check for excel
</commit_message>
<xml_diff>
--- a/Arbeitszeitnachweis Vorlage.xlsx
+++ b/Arbeitszeitnachweis Vorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaa\Documents\work_timer_deta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18880791-7418-457A-BBB9-1E413582109C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EA70C6-9301-43C6-BA8D-DD13324042BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B46B011-59B1-4C45-95D9-6BA23A8D48A8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B46B011-59B1-4C45-95D9-6BA23A8D48A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -719,7 +712,7 @@
   <dimension ref="A1:P497"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +861,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="11"/>
       <c r="F7" s="6" t="str">
-        <f>IF(C7,ROUND((D7-C7-E7)*24,2),"")</f>
+        <f>IF(NOT(ISBLANK(C7)),ROUND((D7-C7-E7)*24,2),"")</f>
         <v/>
       </c>
       <c r="G7" s="11"/>
@@ -892,7 +885,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="11"/>
       <c r="F8" s="6" t="str">
-        <f t="shared" ref="F8:F37" si="0">IF(C8,ROUND((D8-C8-E8)*24,2),"")</f>
+        <f t="shared" ref="F8:F37" si="0">IF(NOT(ISBLANK(C8)),ROUND((D8-C8-E8)*24,2),"")</f>
         <v/>
       </c>
       <c r="G8" s="11"/>

</xml_diff>